<commit_message>
i want comments as practise
</commit_message>
<xml_diff>
--- a/ApplesAndOranges_Unsolved.xlsx
+++ b/ApplesAndOranges_Unsolved.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\reema\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EC45923-F667-4AA4-9596-4B2F05D22B01}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{03302A37-E59C-4E6B-A687-F57B25C89C30}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -446,19 +446,19 @@
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <f ca="1">RANDBETWEEN(1,10)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2">
         <f t="shared" ref="B2:E2" ca="1" si="0">RANDBETWEEN(1,10)</f>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C2">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D2">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E2">
         <f t="shared" ca="1" si="0"/>
@@ -468,11 +468,11 @@
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <f t="shared" ref="A3:E11" ca="1" si="1">RANDBETWEEN(1,10)</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B3">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C3">
         <f t="shared" ca="1" si="1"/>
@@ -480,11 +480,11 @@
       </c>
       <c r="D3">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -498,25 +498,25 @@
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="1"/>
@@ -524,73 +524,73 @@
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="1"/>
@@ -600,11 +600,11 @@
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="1"/>
@@ -612,77 +612,77 @@
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <f ca="1">AVERAGE(A2:A11)</f>
-        <v>4</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="B13" s="1">
         <f t="shared" ref="B13:E13" ca="1" si="2">AVERAGE(B2:B11)</f>
-        <v>6.3</v>
+        <v>6</v>
       </c>
       <c r="C13" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>4.7</v>
+        <v>7.4</v>
       </c>
       <c r="D13" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>6.7</v>
+        <v>5.2</v>
       </c>
       <c r="E13" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>5.8</v>
+        <v>5.6</v>
       </c>
     </row>
   </sheetData>
@@ -696,7 +696,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -727,23 +727,22 @@
       </c>
       <c r="B2">
         <f ca="1">Apples!A13</f>
-        <v>4</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="C2">
         <f ca="1">Apples!B13</f>
-        <v>6.3</v>
+        <v>6</v>
       </c>
       <c r="D2">
         <f ca="1">Apples!C13</f>
-        <v>4.7</v>
+        <v>7.4</v>
       </c>
       <c r="E2">
         <f ca="1">Apples!D13</f>
-        <v>6.7</v>
+        <v>5.2</v>
       </c>
       <c r="F2">
-        <f ca="1">Apples!E13</f>
-        <v>5.8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -752,23 +751,23 @@
       </c>
       <c r="B3">
         <f ca="1">Oranges!A13</f>
-        <v>4.0999999999999996</v>
+        <v>6.1</v>
       </c>
       <c r="C3">
         <f ca="1">Oranges!B13</f>
-        <v>4.3</v>
+        <v>5.6</v>
       </c>
       <c r="D3">
         <f ca="1">Oranges!C13</f>
-        <v>4.5</v>
+        <v>6</v>
       </c>
       <c r="E3">
         <f ca="1">Oranges!D13</f>
-        <v>4.5999999999999996</v>
+        <v>5.6</v>
       </c>
       <c r="F3">
         <f ca="1">Oranges!E13</f>
-        <v>5.8</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -789,7 +788,7 @@
       </c>
       <c r="E4" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>APPLE</v>
+        <v>ORANGES</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -814,7 +813,7 @@
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="1"/>
@@ -894,45 +893,45 @@
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <f ca="1">RANDBETWEEN(1,10)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <f t="shared" ref="B2:E2" ca="1" si="0">RANDBETWEEN(1,10)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D2">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E2">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <f t="shared" ref="A3:E11" ca="1" si="1">RANDBETWEEN(1,10)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B3">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C3">
         <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ca="1" si="1"/>
         <v>8</v>
       </c>
-      <c r="D3">
-        <f t="shared" ca="1" si="1"/>
-        <v>4</v>
-      </c>
       <c r="E3">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -942,103 +941,103 @@
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="1"/>
@@ -1048,89 +1047,89 @@
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="E10">
+        <f t="shared" ca="1" si="1"/>
         <v>10</v>
-      </c>
-      <c r="E10">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <f ca="1">AVERAGE(A2:A11)</f>
-        <v>4.0999999999999996</v>
+        <v>6.1</v>
       </c>
       <c r="B13" s="1">
         <f t="shared" ref="B13:E13" ca="1" si="2">AVERAGE(B2:B11)</f>
-        <v>4.3</v>
+        <v>5.6</v>
       </c>
       <c r="C13" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>4.5</v>
+        <v>6</v>
       </c>
       <c r="D13" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>4.5999999999999996</v>
+        <v>5.6</v>
       </c>
       <c r="E13" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>5.8</v>
+        <v>5.3</v>
       </c>
       <c r="F13" t="s">
         <v>5</v>

</xml_diff>